<commit_message>
updating the code with new prices
</commit_message>
<xml_diff>
--- a/Results/Actual/Actual_EV_rate_cost.xlsx
+++ b/Results/Actual/Actual_EV_rate_cost.xlsx
@@ -31,154 +31,154 @@
     <t>Total Charge</t>
   </si>
   <si>
+    <t>P_1092</t>
+  </si>
+  <si>
+    <t>P_1307</t>
+  </si>
+  <si>
+    <t>P_1111</t>
+  </si>
+  <si>
+    <t>P_1393</t>
+  </si>
+  <si>
+    <t>P_1304</t>
+  </si>
+  <si>
+    <t>P_1279</t>
+  </si>
+  <si>
+    <t>P_1371</t>
+  </si>
+  <si>
+    <t>P_1419</t>
+  </si>
+  <si>
+    <t>P_1421</t>
+  </si>
+  <si>
+    <t>P_1100</t>
+  </si>
+  <si>
+    <t>P_1141</t>
+  </si>
+  <si>
+    <t>P_1093</t>
+  </si>
+  <si>
+    <t>P_1257</t>
+  </si>
+  <si>
+    <t>P_1143</t>
+  </si>
+  <si>
+    <t>P_1272</t>
+  </si>
+  <si>
+    <t>P_1127</t>
+  </si>
+  <si>
+    <t>P_1260</t>
+  </si>
+  <si>
+    <t>P_1123</t>
+  </si>
+  <si>
+    <t>P_1295</t>
+  </si>
+  <si>
+    <t>P_1375</t>
+  </si>
+  <si>
     <t>P_1376</t>
   </si>
   <si>
-    <t>P_1111</t>
-  </si>
-  <si>
-    <t>P_1143</t>
-  </si>
-  <si>
-    <t>P_1127</t>
+    <t>P_1414</t>
+  </si>
+  <si>
+    <t>P_1131</t>
+  </si>
+  <si>
+    <t>P_1112</t>
+  </si>
+  <si>
+    <t>P_1132</t>
+  </si>
+  <si>
+    <t>P_1253</t>
+  </si>
+  <si>
+    <t>P_1135</t>
+  </si>
+  <si>
+    <t>P_1109</t>
+  </si>
+  <si>
+    <t>P_1353</t>
+  </si>
+  <si>
+    <t>P_1424</t>
+  </si>
+  <si>
+    <t>P_1427</t>
+  </si>
+  <si>
+    <t>P_1217</t>
   </si>
   <si>
     <t>P_1271</t>
   </si>
   <si>
-    <t>P_1427</t>
-  </si>
-  <si>
     <t>P_1368</t>
   </si>
   <si>
-    <t>P_1109</t>
-  </si>
-  <si>
-    <t>P_1093</t>
+    <t>P_1094</t>
+  </si>
+  <si>
+    <t>P_1285</t>
+  </si>
+  <si>
+    <t>P_1288</t>
+  </si>
+  <si>
+    <t>P_1357</t>
+  </si>
+  <si>
+    <t>P_1280</t>
+  </si>
+  <si>
+    <t>P_1281</t>
+  </si>
+  <si>
+    <t>P_1296</t>
   </si>
   <si>
     <t>P_1367</t>
   </si>
   <si>
-    <t>P_1414</t>
-  </si>
-  <si>
-    <t>P_1393</t>
-  </si>
-  <si>
-    <t>P_1295</t>
+    <t>P_1125a</t>
   </si>
   <si>
     <t>P_1087</t>
   </si>
   <si>
-    <t>P_1260</t>
+    <t>P_1422</t>
+  </si>
+  <si>
+    <t>P_1137</t>
   </si>
   <si>
     <t>P_1294</t>
   </si>
   <si>
-    <t>P_1131</t>
-  </si>
-  <si>
-    <t>P_1421</t>
-  </si>
-  <si>
-    <t>P_1281</t>
-  </si>
-  <si>
-    <t>P_1092</t>
-  </si>
-  <si>
-    <t>P_1112</t>
-  </si>
-  <si>
-    <t>P_1125a</t>
-  </si>
-  <si>
-    <t>P_1280</t>
-  </si>
-  <si>
-    <t>P_1123</t>
-  </si>
-  <si>
-    <t>P_1253</t>
-  </si>
-  <si>
-    <t>P_1217</t>
-  </si>
-  <si>
-    <t>P_1100</t>
-  </si>
-  <si>
-    <t>P_1353</t>
-  </si>
-  <si>
-    <t>P_1419</t>
-  </si>
-  <si>
-    <t>P_1141</t>
-  </si>
-  <si>
-    <t>P_1288</t>
-  </si>
-  <si>
-    <t>P_1279</t>
-  </si>
-  <si>
-    <t>P_1285</t>
-  </si>
-  <si>
-    <t>P_1422</t>
-  </si>
-  <si>
-    <t>P_1272</t>
+    <t>P_1091</t>
   </si>
   <si>
     <t>P_1125</t>
   </si>
   <si>
-    <t>P_1375</t>
-  </si>
-  <si>
-    <t>P_1137</t>
-  </si>
-  <si>
-    <t>P_1094</t>
-  </si>
-  <si>
-    <t>P_1091</t>
-  </si>
-  <si>
-    <t>P_1296</t>
-  </si>
-  <si>
-    <t>P_1307</t>
-  </si>
-  <si>
-    <t>P_1357</t>
-  </si>
-  <si>
-    <t>P_1371</t>
-  </si>
-  <si>
-    <t>P_1424</t>
-  </si>
-  <si>
-    <t>P_1304</t>
-  </si>
-  <si>
-    <t>P_1257</t>
-  </si>
-  <si>
     <t>P_1098</t>
-  </si>
-  <si>
-    <t>P_1135</t>
-  </si>
-  <si>
-    <t>P_1132</t>
   </si>
 </sst>
 </file>
@@ -567,16 +567,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1548.550016479062</v>
+        <v>2705.384570327582</v>
       </c>
       <c r="D2">
-        <v>93.6871078388067</v>
+        <v>156.3399505236742</v>
       </c>
       <c r="E2">
-        <v>47.39040016173306</v>
+        <v>91.07593037516521</v>
       </c>
       <c r="F2">
-        <v>4248.848428063795</v>
+        <v>7090.247189282279</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -587,16 +587,16 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1186.387800908185</v>
+        <v>1326.101245</v>
       </c>
       <c r="D3">
-        <v>78.49733850000028</v>
+        <v>87.30917999999996</v>
       </c>
       <c r="E3">
-        <v>48.63022563027246</v>
+        <v>53.283533436125</v>
       </c>
       <c r="F3">
-        <v>3559.970000000012</v>
+        <v>3959.599999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -607,16 +607,16 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>1767.097054998311</v>
+        <v>1184.3886825</v>
       </c>
       <c r="D4">
-        <v>100.4333399999997</v>
+        <v>78.49733850000007</v>
       </c>
       <c r="E4">
-        <v>59.92403881084876</v>
+        <v>48.64042827868546</v>
       </c>
       <c r="F4">
-        <v>4554.799999999987</v>
+        <v>3559.970000000003</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -627,16 +627,16 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>3447.00376766666</v>
+        <v>1861.425984098608</v>
       </c>
       <c r="D5">
-        <v>204.9613649999999</v>
+        <v>122.03978091017</v>
       </c>
       <c r="E5">
-        <v>123.2123885862625</v>
+        <v>52.60679542982393</v>
       </c>
       <c r="F5">
-        <v>9295.299999999994</v>
+        <v>5534.68394150431</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -647,16 +647,16 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>3614.315280427593</v>
+        <v>955.8107446153845</v>
       </c>
       <c r="D6">
-        <v>190.3267799999989</v>
+        <v>61.56360000000002</v>
       </c>
       <c r="E6">
-        <v>100.2515404123298</v>
+        <v>36.57289490219227</v>
       </c>
       <c r="F6">
-        <v>8631.599999999951</v>
+        <v>2792</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -667,16 +667,16 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>1657.115414525087</v>
+        <v>2936.149079999988</v>
       </c>
       <c r="D7">
-        <v>98.00278041315676</v>
+        <v>168.40908</v>
       </c>
       <c r="E7">
-        <v>60.23622049201251</v>
+        <v>96.05876624089991</v>
       </c>
       <c r="F7">
-        <v>4444.570540279217</v>
+        <v>7637.599999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -687,16 +687,16 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>1382.507365771743</v>
+        <v>1180.515854016911</v>
       </c>
       <c r="D8">
-        <v>74.43648098050144</v>
+        <v>56.64827908777654</v>
       </c>
       <c r="E8">
-        <v>46.02286255680735</v>
+        <v>33.13819390409638</v>
       </c>
       <c r="F8">
-        <v>3375.804126099838</v>
+        <v>2569.0829518266</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -707,16 +707,16 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>2629.731826319438</v>
+        <v>1232.568295271651</v>
       </c>
       <c r="D9">
-        <v>158.2335562500004</v>
+        <v>67.53164665920092</v>
       </c>
       <c r="E9">
-        <v>98.2265674573776</v>
+        <v>38.6483330356762</v>
       </c>
       <c r="F9">
-        <v>7176.125000000017</v>
+        <v>3062.659712435416</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -727,16 +727,16 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1908.862512697075</v>
+        <v>1157.107673240658</v>
       </c>
       <c r="D10">
-        <v>123.3650092500004</v>
+        <v>65.61978126510103</v>
       </c>
       <c r="E10">
-        <v>76.94205085663299</v>
+        <v>36.30818143506726</v>
       </c>
       <c r="F10">
-        <v>5594.785000000015</v>
+        <v>2975.953798870795</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -747,16 +747,16 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>1422.29931478803</v>
+        <v>2354.434530751681</v>
       </c>
       <c r="D11">
-        <v>83.50570956409044</v>
+        <v>149.7956827499998</v>
       </c>
       <c r="E11">
-        <v>50.11059623959581</v>
+        <v>89.23199304412083</v>
       </c>
       <c r="F11">
-        <v>3787.107009709317</v>
+        <v>6793.454999999992</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -767,16 +767,16 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>762.864850128035</v>
+        <v>3568.465971981511</v>
       </c>
       <c r="D12">
-        <v>45.86764546122762</v>
+        <v>178.5829499999998</v>
       </c>
       <c r="E12">
-        <v>28.6187456631727</v>
+        <v>102.1982032613868</v>
       </c>
       <c r="F12">
-        <v>2080.165327039801</v>
+        <v>8098.999999999988</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -787,16 +787,16 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>1861.416925237027</v>
+        <v>1903.013565189496</v>
       </c>
       <c r="D13">
-        <v>122.03978091017</v>
+        <v>123.3650092500005</v>
       </c>
       <c r="E13">
-        <v>52.60692128736811</v>
+        <v>76.84668256242304</v>
       </c>
       <c r="F13">
-        <v>5534.683941504308</v>
+        <v>5594.785000000023</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -807,16 +807,16 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>1348.385924704662</v>
+        <v>1575.774973634665</v>
       </c>
       <c r="D14">
-        <v>88.51399199999955</v>
+        <v>88.96876707959395</v>
       </c>
       <c r="E14">
-        <v>54.92013124813624</v>
+        <v>53.72884433391435</v>
       </c>
       <c r="F14">
-        <v>4014.239999999979</v>
+        <v>4034.864720162991</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -827,16 +827,16 @@
         <v>18</v>
       </c>
       <c r="C15">
-        <v>3193.09003625579</v>
+        <v>1760.736591886139</v>
       </c>
       <c r="D15">
-        <v>181.5042442499996</v>
+        <v>100.4333399999999</v>
       </c>
       <c r="E15">
-        <v>108.4595392787193</v>
+        <v>59.91512060420938</v>
       </c>
       <c r="F15">
-        <v>8231.484999999982</v>
+        <v>4554.799999999996</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -847,16 +847,16 @@
         <v>19</v>
       </c>
       <c r="C16">
-        <v>2556.445733515166</v>
+        <v>2925.324735442888</v>
       </c>
       <c r="D16">
-        <v>145.7358503319235</v>
+        <v>156.9272040000004</v>
       </c>
       <c r="E16">
-        <v>79.77477318657333</v>
+        <v>94.16916893510829</v>
       </c>
       <c r="F16">
-        <v>6609.33561596025</v>
+        <v>7116.880000000015</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -867,16 +867,16 @@
         <v>20</v>
       </c>
       <c r="C17">
-        <v>732.4806115415737</v>
+        <v>3447.003767666663</v>
       </c>
       <c r="D17">
-        <v>35.58278763351672</v>
+        <v>204.9613649999997</v>
       </c>
       <c r="E17">
-        <v>18.54624877025902</v>
+        <v>123.2169825691001</v>
       </c>
       <c r="F17">
-        <v>1613.73186546561</v>
+        <v>9295.299999999983</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -887,16 +887,16 @@
         <v>21</v>
       </c>
       <c r="C18">
-        <v>2092.359665936377</v>
+        <v>2558.516710438244</v>
       </c>
       <c r="D18">
-        <v>108.7814699999996</v>
+        <v>145.7358503319236</v>
       </c>
       <c r="E18">
-        <v>61.19179832837399</v>
+        <v>79.99428898205711</v>
       </c>
       <c r="F18">
-        <v>4933.399999999981</v>
+        <v>6609.335615960253</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -907,16 +907,16 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>1112.748494047247</v>
+        <v>3313.07877894633</v>
       </c>
       <c r="D19">
-        <v>65.61978126510131</v>
+        <v>138.0354095644854</v>
       </c>
       <c r="E19">
-        <v>36.72348767595176</v>
+        <v>74.6646107620076</v>
       </c>
       <c r="F19">
-        <v>2975.953798870808</v>
+        <v>6260.109277300924</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -927,16 +927,16 @@
         <v>23</v>
       </c>
       <c r="C20">
-        <v>1928.721827217193</v>
+        <v>1347.933576000001</v>
       </c>
       <c r="D20">
-        <v>117.4360950000002</v>
+        <v>88.51399199999986</v>
       </c>
       <c r="E20">
-        <v>68.41988642803443</v>
+        <v>54.93293609434996</v>
       </c>
       <c r="F20">
-        <v>5325.900000000008</v>
+        <v>4014.239999999993</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -947,16 +947,16 @@
         <v>24</v>
       </c>
       <c r="C21">
-        <v>2716.818774505372</v>
+        <v>2300.259317575762</v>
       </c>
       <c r="D21">
-        <v>156.3399505236773</v>
+        <v>120.1460400000001</v>
       </c>
       <c r="E21">
-        <v>90.75728998780227</v>
+        <v>61.20184795059098</v>
       </c>
       <c r="F21">
-        <v>7090.247189282417</v>
+        <v>5448.800000000005</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -967,16 +967,16 @@
         <v>25</v>
       </c>
       <c r="C22">
-        <v>2265.579992136222</v>
+        <v>1549.559821681081</v>
       </c>
       <c r="D22">
-        <v>96.61075199999983</v>
+        <v>93.68710783880661</v>
       </c>
       <c r="E22">
-        <v>44.44015094713687</v>
+        <v>47.30750649483431</v>
       </c>
       <c r="F22">
-        <v>4381.439999999992</v>
+        <v>4248.848428063791</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -987,16 +987,16 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>962.5953413805313</v>
+        <v>762.864850128035</v>
       </c>
       <c r="D23">
-        <v>41.53654878493563</v>
+        <v>45.86764546122762</v>
       </c>
       <c r="E23">
-        <v>20.85836109357214</v>
+        <v>28.6187456631727</v>
       </c>
       <c r="F23">
-        <v>1883.743709067375</v>
+        <v>2080.165327039801</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1007,16 +1007,16 @@
         <v>27</v>
       </c>
       <c r="C24">
-        <v>1094.246760157608</v>
+        <v>2088.648187116987</v>
       </c>
       <c r="D24">
-        <v>66.38461199999995</v>
+        <v>108.7814700000004</v>
       </c>
       <c r="E24">
-        <v>39.5917647233169</v>
+        <v>61.0705177994389</v>
       </c>
       <c r="F24">
-        <v>3010.639999999998</v>
+        <v>4933.400000000017</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1027,16 +1027,16 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>3313.49092269633</v>
+        <v>2262.991851750003</v>
       </c>
       <c r="D25">
-        <v>138.0354095644854</v>
+        <v>96.61075200000002</v>
       </c>
       <c r="E25">
-        <v>74.66732473816386</v>
+        <v>44.59591799591247</v>
       </c>
       <c r="F25">
-        <v>6260.109277300924</v>
+        <v>4381.440000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1047,16 +1047,16 @@
         <v>29</v>
       </c>
       <c r="C26">
-        <v>1081.473647656746</v>
+        <v>1257.320938702072</v>
       </c>
       <c r="D26">
-        <v>54.93316500000052</v>
+        <v>70.53331950000009</v>
       </c>
       <c r="E26">
-        <v>35.07176362812236</v>
+        <v>41.72447031467404</v>
       </c>
       <c r="F26">
-        <v>2491.300000000023</v>
+        <v>3198.790000000004</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1067,16 +1067,16 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>601.9366317763158</v>
+        <v>1078.5775875</v>
       </c>
       <c r="D27">
-        <v>25.47436500000001</v>
+        <v>54.93316500000002</v>
       </c>
       <c r="E27">
-        <v>11.32457645436636</v>
+        <v>35.12202847676254</v>
       </c>
       <c r="F27">
-        <v>1155.3</v>
+        <v>2491.300000000001</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1087,16 +1087,16 @@
         <v>31</v>
       </c>
       <c r="C28">
-        <v>2378.3095441902</v>
+        <v>1868.35710336842</v>
       </c>
       <c r="D28">
-        <v>149.4583177499998</v>
+        <v>118.6907400000003</v>
       </c>
       <c r="E28">
-        <v>88.53451938813961</v>
+        <v>71.40030787805004</v>
       </c>
       <c r="F28">
-        <v>6778.154999999992</v>
+        <v>5382.800000000015</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1107,16 +1107,16 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>1185.9855861992</v>
+        <v>2636.903667083329</v>
       </c>
       <c r="D29">
-        <v>64.09599683416695</v>
+        <v>158.2335562500003</v>
       </c>
       <c r="E29">
-        <v>40.55243436593885</v>
+        <v>98.31126052625729</v>
       </c>
       <c r="F29">
-        <v>2906.847928987163</v>
+        <v>7176.125000000015</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1127,16 +1127,16 @@
         <v>33</v>
       </c>
       <c r="C30">
-        <v>1218.902009567279</v>
+        <v>1187.458966537751</v>
       </c>
       <c r="D30">
-        <v>67.28624309919921</v>
+        <v>64.09599683416663</v>
       </c>
       <c r="E30">
-        <v>39.11625442137719</v>
+        <v>40.58505108367701</v>
       </c>
       <c r="F30">
-        <v>3051.530299283411</v>
+        <v>2906.847928987148</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1147,16 +1147,16 @@
         <v>34</v>
       </c>
       <c r="C31">
-        <v>3562.634234481508</v>
+        <v>367.5125547876154</v>
       </c>
       <c r="D31">
-        <v>178.5829499999998</v>
+        <v>19.65511432815084</v>
       </c>
       <c r="E31">
-        <v>102.1755314373868</v>
+        <v>12.26175685510235</v>
       </c>
       <c r="F31">
-        <v>8098.99999999999</v>
+        <v>891.3884049048</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1167,16 +1167,16 @@
         <v>35</v>
       </c>
       <c r="C32">
-        <v>646.4040912934784</v>
+        <v>1648.670986013978</v>
       </c>
       <c r="D32">
-        <v>38.28530474999996</v>
+        <v>98.43651703802752</v>
       </c>
       <c r="E32">
-        <v>21.57229463952933</v>
+        <v>58.59265312081038</v>
       </c>
       <c r="F32">
-        <v>1736.294999999998</v>
+        <v>4464.241135511452</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1187,16 +1187,16 @@
         <v>36</v>
       </c>
       <c r="C33">
-        <v>2953.093334493983</v>
+        <v>601.1749396710526</v>
       </c>
       <c r="D33">
-        <v>168.40908</v>
+        <v>25.474365</v>
       </c>
       <c r="E33">
-        <v>95.22731745011623</v>
+        <v>11.32326814729268</v>
       </c>
       <c r="F33">
-        <v>7637.599999999999</v>
+        <v>1155.3</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1207,16 +1207,16 @@
         <v>37</v>
       </c>
       <c r="C34">
-        <v>1433.316272637573</v>
+        <v>3616.056223939393</v>
       </c>
       <c r="D34">
-        <v>86.9122799999988</v>
+        <v>190.32678</v>
       </c>
       <c r="E34">
-        <v>50.48069845800737</v>
+        <v>100.2043873143121</v>
       </c>
       <c r="F34">
-        <v>3941.599999999945</v>
+        <v>8631.599999999999</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1227,16 +1227,16 @@
         <v>38</v>
       </c>
       <c r="C35">
-        <v>847.756082760763</v>
+        <v>1383.290288718546</v>
       </c>
       <c r="D35">
-        <v>49.29635530629906</v>
+        <v>74.43648098050134</v>
       </c>
       <c r="E35">
-        <v>28.57584976900786</v>
+        <v>46.05181330529004</v>
       </c>
       <c r="F35">
-        <v>2235.662372167758</v>
+        <v>3375.804126099834</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1247,16 +1247,16 @@
         <v>39</v>
       </c>
       <c r="C36">
-        <v>2918.460615606056</v>
+        <v>2328.450095945075</v>
       </c>
       <c r="D36">
-        <v>156.9272040000002</v>
+        <v>114.314256</v>
       </c>
       <c r="E36">
-        <v>93.99217252099932</v>
+        <v>66.33131540430304</v>
       </c>
       <c r="F36">
-        <v>7116.880000000009</v>
+        <v>5184.319999999997</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1267,16 +1267,16 @@
         <v>40</v>
       </c>
       <c r="C37">
-        <v>877.9569106015655</v>
+        <v>1429.641299999999</v>
       </c>
       <c r="D37">
-        <v>37.52948423153427</v>
+        <v>86.91228000000004</v>
       </c>
       <c r="E37">
-        <v>21.82739817319712</v>
+        <v>50.52206982505907</v>
       </c>
       <c r="F37">
-        <v>1702.017425466407</v>
+        <v>3941.600000000001</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1287,16 +1287,16 @@
         <v>41</v>
       </c>
       <c r="C38">
-        <v>2306.259584242431</v>
+        <v>650.2027944184783</v>
       </c>
       <c r="D38">
-        <v>120.14604</v>
+        <v>38.28530474999997</v>
       </c>
       <c r="E38">
-        <v>61.25813617656539</v>
+        <v>21.60099836996058</v>
       </c>
       <c r="F38">
-        <v>5448.799999999999</v>
+        <v>1736.294999999999</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1307,16 +1307,16 @@
         <v>42</v>
       </c>
       <c r="C39">
-        <v>1607.077580961833</v>
+        <v>1638.316774720954</v>
       </c>
       <c r="D39">
-        <v>78.05541130843675</v>
+        <v>102.2198741718037</v>
       </c>
       <c r="E39">
-        <v>41.08175369102769</v>
+        <v>65.1908425176393</v>
       </c>
       <c r="F39">
-        <v>3539.927950495997</v>
+        <v>4635.821957904929</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1327,16 +1327,16 @@
         <v>43</v>
       </c>
       <c r="C40">
-        <v>2329.356805644214</v>
+        <v>1096.869247090908</v>
       </c>
       <c r="D40">
-        <v>114.3142559999998</v>
+        <v>66.38461199999999</v>
       </c>
       <c r="E40">
-        <v>66.18694343487873</v>
+        <v>39.61473453095603</v>
       </c>
       <c r="F40">
-        <v>5184.319999999991</v>
+        <v>3010.639999999999</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1347,16 +1347,16 @@
         <v>44</v>
       </c>
       <c r="C41">
-        <v>5546.234258583844</v>
+        <v>1932.171259423079</v>
       </c>
       <c r="D41">
-        <v>325.3604287499981</v>
+        <v>117.436095</v>
       </c>
       <c r="E41">
-        <v>200.7572771440708</v>
+        <v>68.50094724358814</v>
       </c>
       <c r="F41">
-        <v>14755.57499999991</v>
+        <v>5325.900000000001</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1367,16 +1367,16 @@
         <v>45</v>
       </c>
       <c r="C42">
-        <v>1747.898982152327</v>
+        <v>1751.640419831837</v>
       </c>
       <c r="D42">
-        <v>88.0302150000005</v>
+        <v>88.03021499999994</v>
       </c>
       <c r="E42">
-        <v>52.18593333594008</v>
+        <v>52.77573966803654</v>
       </c>
       <c r="F42">
-        <v>3992.300000000022</v>
+        <v>3992.299999999997</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1387,16 +1387,16 @@
         <v>46</v>
       </c>
       <c r="C43">
-        <v>1328.138405999999</v>
+        <v>1422.875604374262</v>
       </c>
       <c r="D43">
-        <v>87.30918000000024</v>
+        <v>83.50570956409045</v>
       </c>
       <c r="E43">
-        <v>53.24352530190681</v>
+        <v>50.09945291411204</v>
       </c>
       <c r="F43">
-        <v>3959.600000000011</v>
+        <v>3787.107009709317</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1407,16 +1407,16 @@
         <v>47</v>
       </c>
       <c r="C44">
-        <v>1638.316774720954</v>
+        <v>970.9552616568085</v>
       </c>
       <c r="D44">
-        <v>102.2198741718038</v>
+        <v>41.83201878493561</v>
       </c>
       <c r="E44">
-        <v>65.17710591195542</v>
+        <v>20.95130077938576</v>
       </c>
       <c r="F44">
-        <v>4635.821957904932</v>
+        <v>1897.143709067375</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1427,16 +1427,16 @@
         <v>48</v>
       </c>
       <c r="C45">
-        <v>1122.992824255187</v>
+        <v>3167.998191812507</v>
       </c>
       <c r="D45">
-        <v>56.64827908777661</v>
+        <v>181.5042442499993</v>
       </c>
       <c r="E45">
-        <v>33.26446952163047</v>
+        <v>108.871073795229</v>
       </c>
       <c r="F45">
-        <v>2569.082951826603</v>
+        <v>8231.484999999966</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1447,16 +1447,16 @@
         <v>49</v>
       </c>
       <c r="C46">
-        <v>362.018412690058</v>
+        <v>847.5148239900864</v>
       </c>
       <c r="D46">
-        <v>19.65511432815078</v>
+        <v>49.29635530629912</v>
       </c>
       <c r="E46">
-        <v>12.1597371244724</v>
+        <v>28.5739729539983</v>
       </c>
       <c r="F46">
-        <v>891.3884049047971</v>
+        <v>2235.66237216776</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1467,16 +1467,16 @@
         <v>50</v>
       </c>
       <c r="C47">
-        <v>955.1112081827466</v>
+        <v>1611.088021569844</v>
       </c>
       <c r="D47">
-        <v>61.56360000000087</v>
+        <v>78.35881930843867</v>
       </c>
       <c r="E47">
-        <v>36.56977931767548</v>
+        <v>41.2342618612266</v>
       </c>
       <c r="F47">
-        <v>2792.000000000039</v>
+        <v>3553.687950496084</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1487,16 +1487,16 @@
         <v>51</v>
       </c>
       <c r="C48">
-        <v>1596.094502873189</v>
+        <v>735.9627238962704</v>
       </c>
       <c r="D48">
-        <v>88.96876707959247</v>
+        <v>35.58278763351645</v>
       </c>
       <c r="E48">
-        <v>53.10558576165135</v>
+        <v>18.68265108277637</v>
       </c>
       <c r="F48">
-        <v>4034.864720162923</v>
+        <v>1613.731865465599</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1507,16 +1507,16 @@
         <v>52</v>
       </c>
       <c r="C49">
-        <v>2295.539633423977</v>
+        <v>5574.829652889717</v>
       </c>
       <c r="D49">
-        <v>121.5743120129886</v>
+        <v>325.5459794999994</v>
       </c>
       <c r="E49">
-        <v>58.94050886481674</v>
+        <v>201.0975713303817</v>
       </c>
       <c r="F49">
-        <v>5513.574240951863</v>
+        <v>14763.98999999997</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1527,16 +1527,16 @@
         <v>53</v>
       </c>
       <c r="C50">
-        <v>1873.113868922191</v>
+        <v>878.078724423309</v>
       </c>
       <c r="D50">
-        <v>118.6907399999998</v>
+        <v>37.52948423153453</v>
       </c>
       <c r="E50">
-        <v>71.33348781808063</v>
+        <v>21.83733499788648</v>
       </c>
       <c r="F50">
-        <v>5382.799999999993</v>
+        <v>1702.017425466418</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1547,16 +1547,16 @@
         <v>54</v>
       </c>
       <c r="C51">
-        <v>1259.098077774958</v>
+        <v>2294.152660798979</v>
       </c>
       <c r="D51">
-        <v>70.53331950000057</v>
+        <v>121.5743120129884</v>
       </c>
       <c r="E51">
-        <v>41.503582654459</v>
+        <v>58.89065695678865</v>
       </c>
       <c r="F51">
-        <v>3198.790000000026</v>
+        <v>5513.574240951853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>